<commit_message>
Week1 Day5 w Challenge
</commit_message>
<xml_diff>
--- a/W1 D4 LLM Transformers, Context window, cost and speed comparison.xlsx
+++ b/W1 D4 LLM Transformers, Context window, cost and speed comparison.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\llm_engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E884E3-1CF9-4D54-BEBE-C44819E79096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329979F7-4337-4D5C-B94D-BECEEE0E840A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" activeTab="2" xr2:uid="{FE70412E-462B-470A-99A8-2F1CC5479EF7}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" activeTab="4" xr2:uid="{FE70412E-462B-470A-99A8-2F1CC5479EF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Transformers" sheetId="2" r:id="rId1"/>
     <sheet name="全世界的反應" sheetId="3" r:id="rId2"/>
     <sheet name="Along the Way" sheetId="4" r:id="rId3"/>
     <sheet name="Cost" sheetId="1" r:id="rId4"/>
+    <sheet name="Prompting technology" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Cost!$A$1:$G$29</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="92">
   <si>
     <t>Gemini 2.5 Flash</t>
   </si>
@@ -322,6 +323,78 @@
       <t>），如 GitHub Copilot Workspace</t>
     </r>
   </si>
+  <si>
+    <t>🧠 Prompting 技術整理與比較</t>
+  </si>
+  <si>
+    <t>類型</t>
+  </si>
+  <si>
+    <t>說明</t>
+  </si>
+  <si>
+    <t>範例特點</t>
+  </si>
+  <si>
+    <t>使用情境</t>
+  </si>
+  <si>
+    <t>Zero-shot</t>
+  </si>
+  <si>
+    <t>不提供任何範例，直接給模型任務描述</t>
+  </si>
+  <si>
+    <t>無例子，直接提問</t>
+  </si>
+  <si>
+    <t>任務簡單、模型已熟悉的任務</t>
+  </si>
+  <si>
+    <t>One-shot</t>
+  </si>
+  <si>
+    <t>提供一個範例，讓模型了解任務的格式與期望輸出</t>
+  </si>
+  <si>
+    <t>格式稍複雜、需引導模型思考</t>
+  </si>
+  <si>
+    <t>Multi-shot (Few-shot)</t>
+  </si>
+  <si>
+    <t>提供多個範例，幫助模型學習輸入與輸出的對應模式</t>
+  </si>
+  <si>
+    <t>提供多個 Q&amp;A 或輸入/輸出對應</t>
+  </si>
+  <si>
+    <t>較複雜任務、增加模型準確率</t>
+  </si>
+  <si>
+    <r>
+      <t>提供 1 個</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>輸入與輸出</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>的範例</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -330,7 +403,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,6 +435,13 @@
     <font>
       <i/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -408,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -452,6 +532,16 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -941,7 +1031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32954C9C-DBD1-49F7-960F-EBB14465A7A8}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1705,4 +1795,86 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65F5B641-0E21-412D-AF0E-39CB75B818EA}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.55"/>
+  <cols>
+    <col min="1" max="1" width="22.5" style="21" customWidth="1"/>
+    <col min="2" max="2" width="31.09765625" style="21" customWidth="1"/>
+    <col min="3" max="4" width="31.3984375" style="21" customWidth="1"/>
+    <col min="5" max="16384" width="8.796875" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="22.75">
+      <c r="A1" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="31.05">
+      <c r="A4" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="31.05">
+      <c r="A5" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="31.05">
+      <c r="A6" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>